<commit_message>
MAJ du journal de travail personnel
</commit_message>
<xml_diff>
--- a/Adrien/Journal_Travail.xlsx
+++ b/Adrien/Journal_Travail.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_F7D032B5AE6E561E8C9E2EE3721ACA7E57B54412" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{DDA1D708-1E8E-46D7-B459-F62FC0D359AC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -36,19 +37,31 @@
     <t>Journal de travail</t>
   </si>
   <si>
-    <t>Albert Einstein</t>
-  </si>
-  <si>
-    <t>blablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablabla</t>
-  </si>
-  <si>
-    <t>blablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablabla</t>
+    <t>Adrien Allemand</t>
+  </si>
+  <si>
+    <t>Discution de Groupe du projet</t>
+  </si>
+  <si>
+    <t>Relecture de la synthèse du brainstorming initial</t>
+  </si>
+  <si>
+    <t>Séance de retour sur la proposition du projet</t>
+  </si>
+  <si>
+    <t>Organisation interne suite a la séance de retour</t>
+  </si>
+  <si>
+    <t>spécification du projet, création d'un shéma de dépendence des fonctionalitées</t>
+  </si>
+  <si>
+    <t>Call pour le cahier des charges</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -439,33 +452,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.5546875" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
     </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -476,160 +489,189 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>43150</v>
+        <v>43149</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="8">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>43152</v>
+        <v>43150</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="8">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="8"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="8"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>43157</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>43157</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>43158</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>43163</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="8"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="8"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B32" s="5" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="9">
-        <f>SUM(C5:C31)</f>
-        <v>3</v>
+      <c r="C33" s="9">
+        <f>SUM(C5:C32)</f>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>